<commit_message>
adding lodash to seo see different performance levels
</commit_message>
<xml_diff>
--- a/Javascript/Strings/printReverseData.xlsx
+++ b/Javascript/Strings/printReverseData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abiamvelaquez/Documents/develop/DS and Algos/Javascript/Strings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21D4C5D1-5D5C-054A-8CBF-35B1641018CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2ACB57C-9B61-F34D-83D3-A96A1387965E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="21160" windowHeight="17040" xr2:uid="{2F6C5AB1-ADAD-6B4C-A5AF-93C0C78ED687}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,12 +31,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>looping</t>
   </si>
   <si>
     <t>functions</t>
+  </si>
+  <si>
+    <t>functions with long</t>
+  </si>
+  <si>
+    <t>lodash</t>
   </si>
 </sst>
 </file>
@@ -389,23 +395,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FA2100-B022-CD41-833D-636ACC44AB59}">
-  <dimension ref="B5:I1005"/>
+  <dimension ref="B5:K1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:11">
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:9">
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
       <c r="B6">
         <v>873224</v>
       </c>
@@ -428,7 +440,7 @@
         <v>107811.90399999999</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:11">
       <c r="B7">
         <v>59252</v>
       </c>
@@ -439,7 +451,7 @@
         <v>915802</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:11">
       <c r="B8">
         <v>25203</v>
       </c>
@@ -450,7 +462,7 @@
         <v>187554</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:11">
       <c r="B9">
         <v>26525</v>
       </c>
@@ -461,7 +473,7 @@
         <v>94735</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:11">
       <c r="B10">
         <v>25274</v>
       </c>
@@ -472,7 +484,7 @@
         <v>86882</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:11">
       <c r="B11">
         <v>25149</v>
       </c>
@@ -483,7 +495,7 @@
         <v>112019</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:11">
       <c r="B12">
         <v>25295</v>
       </c>
@@ -494,7 +506,7 @@
         <v>111702</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:11">
       <c r="B13">
         <v>25295</v>
       </c>
@@ -505,7 +517,7 @@
         <v>98870</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:11">
       <c r="B14">
         <v>23891</v>
       </c>
@@ -516,7 +528,7 @@
         <v>111486</v>
       </c>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:11">
       <c r="B15">
         <v>24763</v>
       </c>
@@ -527,7 +539,7 @@
         <v>105496</v>
       </c>
     </row>
-    <row r="16" spans="2:9">
+    <row r="16" spans="2:11">
       <c r="B16">
         <v>19772</v>
       </c>

</xml_diff>

<commit_message>
adding functions to trees in js
</commit_message>
<xml_diff>
--- a/Javascript/Strings/printReverseData.xlsx
+++ b/Javascript/Strings/printReverseData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abiamvelaquez/Documents/develop/DS and Algos/Javascript/Strings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E744E6-DB4B-5A4F-A30E-CADD3871DA9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309640E7-07F2-9B40-A581-1F72ACF24AA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="21160" windowHeight="17040" xr2:uid="{2F6C5AB1-ADAD-6B4C-A5AF-93C0C78ED687}"/>
+    <workbookView xWindow="6120" yWindow="460" windowWidth="21160" windowHeight="17040" xr2:uid="{2F6C5AB1-ADAD-6B4C-A5AF-93C0C78ED687}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,10 +39,10 @@
     <t>functions</t>
   </si>
   <si>
-    <t>functions with long</t>
+    <t>lodash</t>
   </si>
   <si>
-    <t>lodash</t>
+    <t>functions with long on</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="B5:L1005"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -411,10 +411,10 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
         <v>2</v>
-      </c>
-      <c r="K5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:12">

</xml_diff>